<commit_message>
detect loop in a linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DEF7F6-7098-41B6-B230-538EF92F2311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1857,18 +1860,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2413,10 +2416,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="54" spans="1:3">
+      <c r="C54" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="55" spans="1:3" ht="21">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
-      <c r="C55" s="4"/>
+      <c r="C55" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="56" spans="1:3" ht="21">
       <c r="A56" s="5" t="s">
@@ -2891,10 +2901,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="99" spans="1:3">
+      <c r="C99" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="100" spans="1:3" ht="21">
       <c r="A100" s="8"/>
       <c r="B100" s="7"/>
-      <c r="C100" s="4"/>
+      <c r="C100" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="101" spans="1:3" ht="21">
       <c r="A101" s="5" t="s">
@@ -3292,9 +3309,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="137" spans="1:3">
+      <c r="C137" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="138" spans="1:3" ht="21">
       <c r="B138" s="7"/>
-      <c r="C138" s="4"/>
+      <c r="C138" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="139" spans="1:3" ht="21">
       <c r="A139" s="8" t="s">
@@ -3304,7 +3328,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -3315,7 +3339,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">
@@ -3326,7 +3350,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3692,9 +3716,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="175" spans="1:3">
+      <c r="C175" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="176" spans="1:3" ht="21">
       <c r="B176" s="7"/>
-      <c r="C176" s="4"/>
+      <c r="C176" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="177" spans="1:3" ht="21">
       <c r="A177" s="5" t="s">
@@ -4084,12 +4115,16 @@
     <row r="212" spans="1:3" ht="21">
       <c r="A212" s="8"/>
       <c r="B212" s="7"/>
-      <c r="C212" s="4"/>
+      <c r="C212" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="213" spans="1:3" ht="21">
       <c r="A213" s="8"/>
       <c r="B213" s="7"/>
-      <c r="C213" s="4"/>
+      <c r="C213" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="214" spans="1:3" ht="21">
       <c r="A214" s="5" t="s">
@@ -4335,11 +4370,15 @@
     </row>
     <row r="236" spans="1:3" ht="21">
       <c r="B236" s="7"/>
-      <c r="C236" s="4"/>
+      <c r="C236" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="237" spans="1:3" ht="21">
       <c r="B237" s="7"/>
-      <c r="C237" s="4"/>
+      <c r="C237" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="238" spans="1:3" ht="21">
       <c r="A238" s="5" t="s">
@@ -4728,11 +4767,15 @@
     </row>
     <row r="273" spans="1:3" ht="21">
       <c r="B273" s="7"/>
-      <c r="C273" s="4"/>
+      <c r="C273" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="274" spans="1:3" ht="21">
       <c r="B274" s="7"/>
-      <c r="C274" s="4"/>
+      <c r="C274" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="275" spans="1:3" ht="21">
       <c r="A275" s="5" t="s">
@@ -4945,11 +4988,15 @@
     </row>
     <row r="294" spans="1:3" ht="21">
       <c r="B294" s="7"/>
-      <c r="C294" s="4"/>
+      <c r="C294" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="295" spans="1:3" ht="21">
       <c r="B295" s="7"/>
-      <c r="C295" s="4"/>
+      <c r="C295" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="296" spans="1:3" ht="21">
       <c r="A296" s="5" t="s">
@@ -5371,11 +5418,15 @@
     </row>
     <row r="334" spans="1:3" ht="21">
       <c r="B334" s="7"/>
-      <c r="C334" s="4"/>
+      <c r="C334" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="335" spans="1:3" ht="21">
       <c r="B335" s="7"/>
-      <c r="C335" s="4"/>
+      <c r="C335" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="336" spans="1:3" ht="21">
       <c r="A336" s="8" t="s">
@@ -5577,11 +5628,15 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="B354" s="7"/>
-      <c r="C354" s="4"/>
+      <c r="C354" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="B355" s="7"/>
-      <c r="C355" s="4"/>
+      <c r="C355" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="8" t="s">
@@ -6069,11 +6124,15 @@
     </row>
     <row r="400" spans="1:3" ht="21">
       <c r="B400" s="7"/>
-      <c r="C400" s="4"/>
+      <c r="C400" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="401" spans="1:3" ht="21">
       <c r="B401" s="7"/>
-      <c r="C401" s="4"/>
+      <c r="C401" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="402" spans="1:3" ht="21">
       <c r="A402" s="8" t="s">
@@ -6143,11 +6202,15 @@
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="B408" s="7"/>
-      <c r="C408" s="4"/>
+      <c r="C408" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="B409" s="7"/>
-      <c r="C409" s="4"/>
+      <c r="C409" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="5" t="s">
@@ -6811,12 +6874,16 @@
     </row>
     <row r="470" spans="1:3" ht="21">
       <c r="B470" s="7"/>
-      <c r="C470" s="4"/>
+      <c r="C470" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="471" spans="1:3" ht="21">
       <c r="A471" s="8"/>
       <c r="B471" s="7"/>
-      <c r="C471" s="4"/>
+      <c r="C471" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="5" t="s">

</xml_diff>

<commit_message>
delete loop in linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DEF7F6-7098-41B6-B230-538EF92F2311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0390F512-A0FC-4A19-9421-C3E70929A5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F140" sqref="F140"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3361,7 +3361,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">

</xml_diff>

<commit_message>
find starting point of loop
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0390F512-A0FC-4A19-9421-C3E70929A5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BAE871-89D1-4E4F-A590-645DADBA1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H142" sqref="H142"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3372,7 +3372,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">

</xml_diff>

<commit_message>
remove duplicates in a sorted linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BAE871-89D1-4E4F-A590-645DADBA1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6A642C-463A-498F-B255-B794B7F8B406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E142" sqref="E142"/>
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3383,7 +3383,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">

</xml_diff>

<commit_message>
remove duplicates in unsorted linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6A642C-463A-498F-B255-B794B7F8B406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E914EB82-9CDC-4AE3-A6B5-2447146E5127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3394,7 +3394,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">

</xml_diff>

<commit_message>
add 1 to a number represented as a linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E914EB82-9CDC-4AE3-A6B5-2447146E5127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A072D7C-E0C3-4882-891B-5E67524BEBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E143" sqref="E143"/>
+      <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3405,7 +3405,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">

</xml_diff>

<commit_message>
add 2 numbrs represented as linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A072D7C-E0C3-4882-891B-5E67524BEBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C970E0A-2B1F-47EC-8281-EDBD6E8451F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E145" sqref="E145"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3416,7 +3416,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">
@@ -3427,7 +3427,7 @@
         <v>144</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21">

</xml_diff>

<commit_message>
intersection of two sorted linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C970E0A-2B1F-47EC-8281-EDBD6E8451F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D5001E-7848-490A-987F-ACECFF769AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3438,7 +3438,7 @@
         <v>145</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21">

</xml_diff>

<commit_message>
intersection point of two linked lists
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D5001E-7848-490A-987F-ACECFF769AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F83ADCB-EC83-4CFC-8070-523D09F959A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+      <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3449,7 +3449,7 @@
         <v>146</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="21">

</xml_diff>

<commit_message>
merge sort for linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F83ADCB-EC83-4CFC-8070-523D09F959A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8B133F-BA33-4892-8ABA-3CE75B0428E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3460,7 +3460,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">

</xml_diff>

<commit_message>
quick sort for linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8B133F-BA33-4892-8ABA-3CE75B0428E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8D1E7E-F0EA-4276-8666-1EE9E5CABFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3471,7 +3471,7 @@
         <v>148</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21">

</xml_diff>

<commit_message>
find the middle element of a linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8D1E7E-F0EA-4276-8666-1EE9E5CABFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC874949-8BE5-460F-9D96-73F6EDA0247A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3482,7 +3482,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="21">

</xml_diff>

<commit_message>
split circular linked list into two halves
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EB8FB5-6596-4DF0-9BF2-11A0436D430F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAC71F2-7ED8-48E7-81D4-303CD93D23CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3504,7 +3504,7 @@
         <v>151</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="21">

</xml_diff>

<commit_message>
deletion from circular linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAC71F2-7ED8-48E7-81D4-303CD93D23CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD09115D-FD5B-4810-8877-6D1A8906F95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3515,7 +3515,7 @@
         <v>152</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="21">
@@ -3526,7 +3526,7 @@
         <v>153</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="21">

</xml_diff>

<commit_message>
find pairs with a given sum in sorted doubly linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD09115D-FD5B-4810-8877-6D1A8906F95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826F9A5C-25A7-46EC-872B-32AB2D3B6ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C158" sqref="C158"/>
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3537,7 +3537,7 @@
         <v>154</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21">
@@ -3548,7 +3548,7 @@
         <v>155</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21">

</xml_diff>

<commit_message>
sort a k sorted doubly linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826F9A5C-25A7-46EC-872B-32AB2D3B6ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2318E7-160D-4B9D-B73F-5582A0120546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3559,7 +3559,7 @@
         <v>156</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="21">
@@ -3570,7 +3570,7 @@
         <v>157</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="21">

</xml_diff>

<commit_message>
rotate doubly linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2318E7-160D-4B9D-B73F-5582A0120546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF26693A-404C-4112-B3D9-CBED77976F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F209" sqref="F209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3581,7 +3581,7 @@
         <v>158</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21">

</xml_diff>

<commit_message>
reverse doubly linked list in size of k
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF26693A-404C-4112-B3D9-CBED77976F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC88855-F20F-49D9-8546-0D25744E37B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F209" sqref="F209"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3592,7 +3592,7 @@
         <v>159</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21">
@@ -3717,15 +3717,11 @@
       </c>
     </row>
     <row r="175" spans="1:3">
-      <c r="C175" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C175" s="4"/>
     </row>
     <row r="176" spans="1:3" ht="21">
       <c r="B176" s="7"/>
-      <c r="C176" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C176" s="4"/>
     </row>
     <row r="177" spans="1:3" ht="21">
       <c r="A177" s="5" t="s">

</xml_diff>

<commit_message>
sort a linked list of 0's, 1's and 2's
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC88855-F20F-49D9-8546-0D25744E37B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E477E5A-6BD4-4566-B775-61B0FD1AF4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3625,7 +3625,7 @@
         <v>162</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="21">
@@ -3636,7 +3636,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21">

</xml_diff>

<commit_message>
clone a linked list with next and random pointer
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E477E5A-6BD4-4566-B775-61B0FD1AF4BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269FD8DE-8FDC-45A1-9DD1-7FDE3206DBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3647,7 +3647,7 @@
         <v>164</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="21">

</xml_diff>

<commit_message>
multiply two numbers represented as linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269FD8DE-8FDC-45A1-9DD1-7FDE3206DBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B4CEE8-7ED5-429F-AAA7-3BA6A4B3062B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3658,7 +3658,7 @@
         <v>165</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="21">
@@ -3669,7 +3669,7 @@
         <v>166</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="21">

</xml_diff>

<commit_message>
delete nodes which have a greater value on right side
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B4CEE8-7ED5-429F-AAA7-3BA6A4B3062B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD37E28-AB00-40C0-9ABC-40B28CF58D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3680,7 +3680,7 @@
         <v>167</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="21">

</xml_diff>

<commit_message>
segregate even and odd nodes in a linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD37E28-AB00-40C0-9ABC-40B28CF58D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E686F7-C82F-42B0-96D1-A65B75208CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3691,7 +3691,7 @@
         <v>168</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="21">

</xml_diff>

<commit_message>
get the nth node from the end of linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E686F7-C82F-42B0-96D1-A65B75208CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF4AFD-19D6-40F2-A273-F798DF84A8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3702,7 +3702,7 @@
         <v>169</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="21">
@@ -3713,7 +3713,7 @@
         <v>170</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="175" spans="1:3">

</xml_diff>

<commit_message>
reverse level order traversal
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988F46D4-8CF0-4BB0-9C57-9F3290488ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78521EBE-A240-4F92-A761-21A1ED5643F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3742,7 +3742,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">

</xml_diff>

<commit_message>
diameter of a binary tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78521EBE-A240-4F92-A761-21A1ED5643F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52271F02-15BD-4CCD-8045-2CC68AB79CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3764,7 +3764,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">

</xml_diff>

<commit_message>
right view of tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A58602E-DF7F-4378-835D-CC3206E995EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9867C7B-D0D3-4907-825F-0E964D1B61B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F181" sqref="F181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3808,7 +3808,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -3819,7 +3819,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3830,7 +3830,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">

</xml_diff>

<commit_message>
top view of tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9867C7B-D0D3-4907-825F-0E964D1B61B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188BF329-2A7A-4F3A-A401-A2BFA45C6961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F181" sqref="F181"/>
+    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3841,7 +3841,7 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">

</xml_diff>

<commit_message>
bottom view of tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188BF329-2A7A-4F3A-A401-A2BFA45C6961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0826B412-B6B4-487C-B79B-AB03E8D6D1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -3852,7 +3852,7 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">

</xml_diff>

<commit_message>
zig-zag traversal of tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0826B412-B6B4-487C-B79B-AB03E8D6D1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D6A195-A7FD-4E14-9C0B-5702C118B726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C188" sqref="C188"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3863,7 +3863,7 @@
         <v>184</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">

</xml_diff>

<commit_message>
check if tree is balanced
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D6A195-A7FD-4E14-9C0B-5702C118B726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0B12BA-D90E-4504-9B97-458CC03E911F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3874,7 +3874,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">

</xml_diff>

<commit_message>
construct binary tree from string
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2008421E-9CD9-4C03-ADE6-5F7433188608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632A0E5D-323F-4493-889C-C3496CF6A23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A171" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D189" sqref="D189"/>
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3907,7 +3907,7 @@
         <v>188</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="21">

</xml_diff>

<commit_message>
check whether binary tree is a sum or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632A0E5D-323F-4493-889C-C3496CF6A23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF305F3C-E8D0-49B2-A171-197EF6FCDEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C193" sqref="C193"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C199" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3918,7 +3918,7 @@
         <v>189</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="21">
@@ -3929,7 +3929,7 @@
         <v>190</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="21">
@@ -3951,7 +3951,7 @@
         <v>192</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="21">
@@ -3962,7 +3962,7 @@
         <v>193</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="21">

</xml_diff>

<commit_message>
check if the leaves in a bt are at the same level or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF305F3C-E8D0-49B2-A171-197EF6FCDEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619D3F63-02BF-443F-9BB5-C93213FAFFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C199" sqref="C199"/>
+    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3973,7 +3973,7 @@
         <v>194</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="21">

</xml_diff>

<commit_message>
check mirror in two n-ary trees
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619D3F63-02BF-443F-9BB5-C93213FAFFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12420CD-BF13-4F9C-AC1E-6C4EC7C3ECF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A198" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+      <selection activeCell="D211" sqref="D211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3984,7 +3984,7 @@
         <v>195</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="21">
@@ -3995,7 +3995,7 @@
         <v>196</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="21">

</xml_diff>

<commit_message>
check if given graph is tree or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12420CD-BF13-4F9C-AC1E-6C4EC7C3ECF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DC187B-5E7C-4DE6-BB2C-FA0B357096BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D211" sqref="D211"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B204" sqref="B204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -4006,7 +4006,7 @@
         <v>197</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="21">
@@ -4017,7 +4017,7 @@
         <v>198</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="21">

</xml_diff>

<commit_message>
get largest subtree sum
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DC187B-5E7C-4DE6-BB2C-FA0B357096BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0446DD-8DEF-4C9D-8ADB-E4AC3E264064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A190" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B204" sqref="B204"/>
+      <selection activeCell="C205" sqref="C205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -4028,7 +4028,7 @@
         <v>199</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="21">

</xml_diff>

<commit_message>
construct tree from preorder and inorder(needs changes)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0446DD-8DEF-4C9D-8ADB-E4AC3E264064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A61AC-9BC7-439E-A1AB-42437F1AD856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C205" sqref="C205"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C208" sqref="C208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -4039,7 +4039,7 @@
         <v>200</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="21">
@@ -4050,7 +4050,7 @@
         <v>201</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="21">
@@ -4061,7 +4061,7 @@
         <v>202</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="21">
@@ -4072,7 +4072,7 @@
         <v>203</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="21">

</xml_diff>

<commit_message>
kth ancestor of a node in bt
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Pc\Desktop\DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A61AC-9BC7-439E-A1AB-42437F1AD856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1542773D-A11E-4BA5-95A0-1D2DF79D44F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1860,18 +1860,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C210" sqref="C210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25">
+    <row r="1" spans="1:3" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>204</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="21">

</xml_diff>

<commit_message>
find all duplicate subtrees in a binary tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1542773D-A11E-4BA5-95A0-1D2DF79D44F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2398F422-68AA-4D8D-B927-2931E57569D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -4094,7 +4094,7 @@
         <v>205</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="21">

</xml_diff>

<commit_message>
topological sort code changed
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBED45D-C3A3-4044-98C2-9757BC02D3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF26BBE1-7067-4324-B801-A2458585B31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1432,6 +1432,9 @@
   </si>
   <si>
     <t>Tried multiple times</t>
+  </si>
+  <si>
+    <t>Hamiltonian cycle</t>
   </si>
 </sst>
 </file>
@@ -1870,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:D481"/>
+  <dimension ref="A1:D482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C368" sqref="C368"/>
+    <sheetView tabSelected="1" topLeftCell="A378" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C400" sqref="A400:C400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
@@ -5722,7 +5725,7 @@
         <v>350</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="363" spans="1:3" ht="21">
@@ -5821,7 +5824,7 @@
         <v>359</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="21">
@@ -5832,7 +5835,7 @@
         <v>360</v>
       </c>
       <c r="C372" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="373" spans="1:3" ht="21">
@@ -5843,7 +5846,7 @@
         <v>361</v>
       </c>
       <c r="C373" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="374" spans="1:3" ht="21">
@@ -5854,7 +5857,7 @@
         <v>362</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="375" spans="1:3" ht="21">
@@ -5876,7 +5879,7 @@
         <v>364</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="377" spans="1:3" ht="21">
@@ -5887,7 +5890,7 @@
         <v>365</v>
       </c>
       <c r="C377" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="378" spans="1:3" ht="21">
@@ -5942,7 +5945,7 @@
         <v>370</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="383" spans="1:3" ht="21">
@@ -5953,18 +5956,18 @@
         <v>371</v>
       </c>
       <c r="C383" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="384" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" ht="19.5">
       <c r="A384" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="B384" s="6" t="s">
+      <c r="B384" s="10" t="s">
         <v>372</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="385" spans="1:3" ht="21">
@@ -6133,7 +6136,12 @@
       </c>
     </row>
     <row r="400" spans="1:3" ht="21">
-      <c r="B400" s="7"/>
+      <c r="A400" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B400" s="6" t="s">
+        <v>467</v>
+      </c>
       <c r="C400" s="4" t="s">
         <v>4</v>
       </c>
@@ -6145,12 +6153,7 @@
       </c>
     </row>
     <row r="402" spans="1:3" ht="21">
-      <c r="A402" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="B402" s="6" t="s">
-        <v>388</v>
-      </c>
+      <c r="B402" s="7"/>
       <c r="C402" s="4" t="s">
         <v>4</v>
       </c>
@@ -6160,7 +6163,7 @@
         <v>387</v>
       </c>
       <c r="B403" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C403" s="4" t="s">
         <v>4</v>
@@ -6171,7 +6174,7 @@
         <v>387</v>
       </c>
       <c r="B404" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C404" s="4" t="s">
         <v>4</v>
@@ -6182,7 +6185,7 @@
         <v>387</v>
       </c>
       <c r="B405" s="6" t="s">
-        <v>89</v>
+        <v>390</v>
       </c>
       <c r="C405" s="4" t="s">
         <v>4</v>
@@ -6193,7 +6196,7 @@
         <v>387</v>
       </c>
       <c r="B406" s="6" t="s">
-        <v>391</v>
+        <v>89</v>
       </c>
       <c r="C406" s="4" t="s">
         <v>4</v>
@@ -6204,14 +6207,19 @@
         <v>387</v>
       </c>
       <c r="B407" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C407" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" ht="21">
+      <c r="A408" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B408" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="C407" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="408" spans="1:3" ht="21">
-      <c r="B408" s="7"/>
       <c r="C408" s="4" t="s">
         <v>4</v>
       </c>
@@ -6223,12 +6231,7 @@
       </c>
     </row>
     <row r="410" spans="1:3" ht="21">
-      <c r="A410" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="B410" s="6" t="s">
-        <v>394</v>
-      </c>
+      <c r="B410" s="7"/>
       <c r="C410" s="4" t="s">
         <v>4</v>
       </c>
@@ -6238,7 +6241,7 @@
         <v>393</v>
       </c>
       <c r="B411" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C411" s="4" t="s">
         <v>4</v>
@@ -6249,7 +6252,7 @@
         <v>393</v>
       </c>
       <c r="B412" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C412" s="4" t="s">
         <v>4</v>
@@ -6260,7 +6263,7 @@
         <v>393</v>
       </c>
       <c r="B413" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C413" s="4" t="s">
         <v>4</v>
@@ -6271,7 +6274,7 @@
         <v>393</v>
       </c>
       <c r="B414" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C414" s="4" t="s">
         <v>4</v>
@@ -6282,7 +6285,7 @@
         <v>393</v>
       </c>
       <c r="B415" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C415" s="4" t="s">
         <v>4</v>
@@ -6293,7 +6296,7 @@
         <v>393</v>
       </c>
       <c r="B416" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C416" s="4" t="s">
         <v>4</v>
@@ -6304,7 +6307,7 @@
         <v>393</v>
       </c>
       <c r="B417" s="6" t="s">
-        <v>273</v>
+        <v>400</v>
       </c>
       <c r="C417" s="4" t="s">
         <v>4</v>
@@ -6315,7 +6318,7 @@
         <v>393</v>
       </c>
       <c r="B418" s="6" t="s">
-        <v>401</v>
+        <v>273</v>
       </c>
       <c r="C418" s="4" t="s">
         <v>4</v>
@@ -6326,7 +6329,7 @@
         <v>393</v>
       </c>
       <c r="B419" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C419" s="4" t="s">
         <v>4</v>
@@ -6337,7 +6340,7 @@
         <v>393</v>
       </c>
       <c r="B420" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C420" s="4" t="s">
         <v>4</v>
@@ -6348,7 +6351,7 @@
         <v>393</v>
       </c>
       <c r="B421" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C421" s="4" t="s">
         <v>4</v>
@@ -6359,7 +6362,7 @@
         <v>393</v>
       </c>
       <c r="B422" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C422" s="4" t="s">
         <v>4</v>
@@ -6370,7 +6373,7 @@
         <v>393</v>
       </c>
       <c r="B423" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C423" s="4" t="s">
         <v>4</v>
@@ -6381,7 +6384,7 @@
         <v>393</v>
       </c>
       <c r="B424" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C424" s="4" t="s">
         <v>4</v>
@@ -6392,7 +6395,7 @@
         <v>393</v>
       </c>
       <c r="B425" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C425" s="4" t="s">
         <v>4</v>
@@ -6403,7 +6406,7 @@
         <v>393</v>
       </c>
       <c r="B426" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C426" s="4" t="s">
         <v>4</v>
@@ -6414,7 +6417,7 @@
         <v>393</v>
       </c>
       <c r="B427" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C427" s="4" t="s">
         <v>4</v>
@@ -6425,7 +6428,7 @@
         <v>393</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C428" s="4" t="s">
         <v>4</v>
@@ -6436,7 +6439,7 @@
         <v>393</v>
       </c>
       <c r="B429" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C429" s="4" t="s">
         <v>4</v>
@@ -6447,7 +6450,7 @@
         <v>393</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C430" s="4" t="s">
         <v>4</v>
@@ -6458,7 +6461,7 @@
         <v>393</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C431" s="4" t="s">
         <v>4</v>
@@ -6469,7 +6472,7 @@
         <v>393</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C432" s="4" t="s">
         <v>4</v>
@@ -6480,7 +6483,7 @@
         <v>393</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>4</v>
@@ -6491,7 +6494,7 @@
         <v>393</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>4</v>
@@ -6502,7 +6505,7 @@
         <v>393</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>4</v>
@@ -6513,7 +6516,7 @@
         <v>393</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6524,7 +6527,7 @@
         <v>393</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6535,7 +6538,7 @@
         <v>393</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6546,7 +6549,7 @@
         <v>393</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6557,7 +6560,7 @@
         <v>393</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6568,7 +6571,7 @@
         <v>393</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6579,7 +6582,7 @@
         <v>393</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6590,7 +6593,7 @@
         <v>393</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6601,7 +6604,7 @@
         <v>393</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C444" s="4" t="s">
         <v>4</v>
@@ -6612,7 +6615,7 @@
         <v>393</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6623,7 +6626,7 @@
         <v>393</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6634,7 +6637,7 @@
         <v>393</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6645,7 +6648,7 @@
         <v>393</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6656,7 +6659,7 @@
         <v>393</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6667,7 +6670,7 @@
         <v>393</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6678,7 +6681,7 @@
         <v>393</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6689,7 +6692,7 @@
         <v>393</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C452" s="4" t="s">
         <v>4</v>
@@ -6700,7 +6703,7 @@
         <v>393</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6711,7 +6714,7 @@
         <v>393</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6722,7 +6725,7 @@
         <v>393</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6733,7 +6736,7 @@
         <v>393</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6744,7 +6747,7 @@
         <v>393</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6755,7 +6758,7 @@
         <v>393</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6766,7 +6769,7 @@
         <v>393</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6777,7 +6780,7 @@
         <v>393</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -6788,7 +6791,7 @@
         <v>393</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -6799,7 +6802,7 @@
         <v>393</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -6810,7 +6813,7 @@
         <v>393</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -6821,7 +6824,7 @@
         <v>393</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -6832,7 +6835,7 @@
         <v>393</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -6843,7 +6846,7 @@
         <v>393</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -6854,7 +6857,7 @@
         <v>393</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -6865,7 +6868,7 @@
         <v>393</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -6876,32 +6879,32 @@
         <v>393</v>
       </c>
       <c r="B469" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C469" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" ht="21">
+      <c r="A470" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B470" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="C469" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="470" spans="1:3" ht="21">
-      <c r="B470" s="7"/>
       <c r="C470" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="471" spans="1:3" ht="21">
-      <c r="A471" s="8"/>
       <c r="B471" s="7"/>
       <c r="C471" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="472" spans="1:3" ht="21">
-      <c r="A472" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="B472" s="6" t="s">
-        <v>454</v>
-      </c>
+      <c r="A472" s="8"/>
+      <c r="B472" s="7"/>
       <c r="C472" s="4" t="s">
         <v>4</v>
       </c>
@@ -6911,7 +6914,7 @@
         <v>453</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C473" s="4" t="s">
         <v>4</v>
@@ -6922,7 +6925,7 @@
         <v>453</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C474" s="4" t="s">
         <v>4</v>
@@ -6933,7 +6936,7 @@
         <v>453</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C475" s="4" t="s">
         <v>4</v>
@@ -6944,7 +6947,7 @@
         <v>453</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C476" s="4" t="s">
         <v>4</v>
@@ -6955,7 +6958,7 @@
         <v>453</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C477" s="4" t="s">
         <v>4</v>
@@ -6966,7 +6969,7 @@
         <v>453</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C478" s="4" t="s">
         <v>4</v>
@@ -6977,7 +6980,7 @@
         <v>453</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C479" s="4" t="s">
         <v>4</v>
@@ -6988,7 +6991,7 @@
         <v>453</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C480" s="4" t="s">
         <v>4</v>
@@ -6999,9 +7002,20 @@
         <v>453</v>
       </c>
       <c r="B481" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="C481" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" ht="21">
+      <c r="A482" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B482" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="C481" s="4" t="s">
+      <c r="C482" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7375,82 +7389,82 @@
     <hyperlink ref="B397" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
     <hyperlink ref="B398" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
     <hyperlink ref="B399" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B402" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B403" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B404" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B405" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B406" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B407" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B410" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B411" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B412" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B413" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B414" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B415" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B416" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B417" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B418" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B419" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B420" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B421" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B422" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B423" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B424" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B425" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B426" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B427" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B428" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B429" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B430" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B431" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B432" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B433" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B434" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B435" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B436" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B437" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B438" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B439" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B440" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B441" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B442" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B443" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B444" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B445" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B446" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B447" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B448" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B449" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B451" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B450" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B452" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B453" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B454" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B455" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B456" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B457" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B458" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B459" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B460" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B461" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B462" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B469" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B468" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B467" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B466" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B465" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B464" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B463" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B472" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B473" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B474" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B475" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B476" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B477" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B478" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B481" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B479" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B403" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B404" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B405" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B406" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B407" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B408" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B411" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B412" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B413" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B414" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B415" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B416" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B417" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B418" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B419" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B420" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B421" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B422" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B423" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B424" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B425" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B426" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B427" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B428" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B429" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B430" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B431" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B432" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B433" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B434" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B435" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B436" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B437" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B438" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B439" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B440" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B441" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B442" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B443" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B444" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B445" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B446" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B447" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B448" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B449" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B450" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B452" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B451" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B453" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B454" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B455" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B456" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B457" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B458" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B459" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B460" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B461" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B462" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B463" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B470" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B469" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B468" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B467" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B466" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B465" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B464" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B473" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B474" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B475" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B476" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B477" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B478" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B479" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B482" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B480" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B481" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
     <hyperlink ref="B356" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
max and min elements in array with min comparisons
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF9EAE4-D826-4014-B09C-0A902B6B7369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B938F9-EF0F-4354-974B-81C21128233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1916,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">

</xml_diff>

<commit_message>
kth smallest element in unsorted array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B938F9-EF0F-4354-974B-81C21128233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9D6621-4D6A-4ECD-907F-0FC722A63065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1927,7 +1927,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">

</xml_diff>

<commit_message>
sort array with 0, 1 and 2
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9D6621-4D6A-4ECD-907F-0FC722A63065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82446C69-218A-4928-8D6D-AE398CFDD664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1938,7 +1938,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">

</xml_diff>

<commit_message>
move negative elements to the beginning of the array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82446C69-218A-4928-8D6D-AE398CFDD664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50837593-158B-4C3A-BA30-2928CFD76379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1949,7 +1949,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">

</xml_diff>

<commit_message>
find union and intersection of two arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50837593-158B-4C3A-BA30-2928CFD76379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB678341-E59E-45F2-9DB4-9E15BD9EA5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1960,7 +1960,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">

</xml_diff>

<commit_message>
cyclically rotate an array by one
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB678341-E59E-45F2-9DB4-9E15BD9EA5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3291D817-3139-490F-B9B0-0E5C91500596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1971,7 +1971,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">

</xml_diff>

<commit_message>
largest contiguous subarray sum
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3291D817-3139-490F-B9B0-0E5C91500596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5113C6E4-1170-414E-82EB-5B1405E58DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1982,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">

</xml_diff>

<commit_message>
find duplicate in an array of n+1 integers
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5113C6E4-1170-414E-82EB-5B1405E58DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CB30B1-3B17-4A6E-A9B6-41722E613B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2015,7 +2015,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">

</xml_diff>

<commit_message>
merge two arrays without using extra space
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CB30B1-3B17-4A6E-A9B6-41722E613B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEC4B5E-3DFE-42D8-8CB7-5DDAA96BDF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2026,7 +2026,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2037,7 +2037,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2048,7 +2048,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">

</xml_diff>

<commit_message>
common element in 3 sorted arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEC4B5E-3DFE-42D8-8CB7-5DDAA96BDF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE732EB0-F930-4CC5-A314-9CC5A58BD3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1429,6 +1429,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TYPICAL</t>
   </si>
 </sst>
 </file>
@@ -1858,10 +1861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1871,17 +1874,17 @@
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25">
+    <row r="1" spans="1:4" ht="25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="B2" s="10" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21">
+    <row r="4" spans="1:4" ht="21">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1892,12 +1895,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21">
+    <row r="6" spans="1:4" ht="21">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21">
+    <row r="7" spans="1:4" ht="21">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21">
+    <row r="8" spans="1:4" ht="21">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21">
+    <row r="9" spans="1:4" ht="21">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21">
+    <row r="10" spans="1:4" ht="21">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1952,7 +1955,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21">
+    <row r="11" spans="1:4" ht="21">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21">
+    <row r="12" spans="1:4" ht="21">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21">
+    <row r="13" spans="1:4" ht="21">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21">
+    <row r="14" spans="1:4" ht="21">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21">
+    <row r="15" spans="1:4" ht="21">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2006,8 +2009,11 @@
       <c r="C15" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="21">
+      <c r="D15" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="21">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2018,7 +2024,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21">
+    <row r="17" spans="1:4" ht="21">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21">
+    <row r="18" spans="1:4" ht="21">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2040,7 +2046,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21">
+    <row r="19" spans="1:4" ht="21">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21">
+    <row r="20" spans="1:4" ht="21">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -2061,8 +2067,11 @@
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="21">
+      <c r="D20" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="21">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2073,7 +2082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21">
+    <row r="22" spans="1:4" ht="21">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21">
+    <row r="23" spans="1:4" ht="21">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2095,7 +2104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21">
+    <row r="24" spans="1:4" ht="21">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -2103,10 +2112,10 @@
         <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="21">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
@@ -2117,7 +2126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21">
+    <row r="26" spans="1:4" ht="21">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -2125,10 +2134,10 @@
         <v>26</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="21">
       <c r="A27" s="5" t="s">
         <v>5</v>
       </c>
@@ -2136,10 +2145,10 @@
         <v>27</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="21">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21">
       <c r="A28" s="5" t="s">
         <v>5</v>
       </c>
@@ -2150,7 +2159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21">
+    <row r="29" spans="1:4" ht="21">
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
@@ -2161,7 +2170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21">
+    <row r="30" spans="1:4" ht="21">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -2172,7 +2181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21">
+    <row r="31" spans="1:4" ht="21">
       <c r="A31" s="5" t="s">
         <v>5</v>
       </c>
@@ -2183,7 +2192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21">
+    <row r="32" spans="1:4" ht="21">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
min swaps and k together
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6115512C-E7D9-454C-9A30-B65AEF27E620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AF8DC1-6CAA-4804-A5E6-3FF6C65622AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="470">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1438,6 +1438,9 @@
   </si>
   <si>
     <t>https://youtu.be/PwEdhxQkFZs</t>
+  </si>
+  <si>
+    <t>https://youtu.be/yXjVfeWzyAM</t>
   </si>
 </sst>
 </file>
@@ -1870,7 +1873,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2278,7 +2281,10 @@
         <v>38</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
+      </c>
+      <c r="D38" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="21">

</xml_diff>